<commit_message>
Fix urls in xml
Fix url in resource xml from /max-fhir-ru/StructureDefinition/Encounter to /max-fhir-ru/StructureDefinition-Encounter
</commit_message>
<xml_diff>
--- a/StructureDefinition-Encounter.xlsx
+++ b/StructureDefinition-Encounter.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://maximnikolaev.github.io/max-fhir-ru/StructureDefinition/Encounter</t>
+    <t>https://maximnikolaev.github.io/max-fhir-ru/StructureDefinition-Encounter</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-06-17T16:49:09+03:00</t>
+    <t>2022-06-17T17:13:24+03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>